<commit_message>
[IMP] add c++ template
</commit_message>
<xml_diff>
--- a/src/main/resources/script/db/init-data/devops_service/devops_service/devops_app_template.xlsx
+++ b/src/main/resources/script/db/init-data/devops_service/devops_service/devops_app_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="19420" tabRatio="597" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="12090" tabRatio="597" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="115">
   <si>
     <r>
       <rPr>
@@ -2167,6 +2167,18 @@
   </si>
   <si>
     <t>基于.NET Framework的Web开发模版（一般用于创建普通类型应用服务）</t>
+  </si>
+  <si>
+    <t>devops_app_template-12</t>
+  </si>
+  <si>
+    <t>C/C++Template</t>
+  </si>
+  <si>
+    <t>ctemplate</t>
+  </si>
+  <si>
+    <t>c/c++开发模板</t>
   </si>
 </sst>
 </file>
@@ -2175,9 +2187,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="38">
     <font>
@@ -2225,12 +2237,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="DengXian"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color rgb="FFC55A11"/>
       <name val="DengXian"/>
       <charset val="134"/>
@@ -2248,18 +2254,10 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="DengXian"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2269,7 +2267,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
@@ -2294,14 +2291,35 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2309,7 +2327,22 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2323,19 +2356,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
       <name val="等线"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2355,35 +2388,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -2392,8 +2396,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2475,13 +2487,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2493,19 +2553,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2523,19 +2643,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2547,115 +2661,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2672,28 +2684,12 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -2718,12 +2714,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
+      <right/>
+      <top style="thin">
         <color auto="1"/>
-      </right>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -2735,20 +2749,18 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top/>
-      <bottom style="thin">
+      <top style="thin">
         <color auto="1"/>
-      </bottom>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
+      <left style="thin">
         <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      </left>
+      <right/>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -2765,19 +2777,47 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2786,7 +2826,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2821,200 +2861,175 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="30" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="31" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="12" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3025,112 +3040,112 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 2" xfId="1"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="2" builtinId="52"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="3" builtinId="42"/>
-    <cellStyle name="强调文字颜色 4" xfId="4" builtinId="41"/>
-    <cellStyle name="输入" xfId="5" builtinId="20"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
     <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="7" builtinId="38"/>
-    <cellStyle name="货币" xfId="8" builtinId="4"/>
-    <cellStyle name="强调文字颜色 3" xfId="9" builtinId="37"/>
-    <cellStyle name="百分比" xfId="10" builtinId="5"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="11" builtinId="36"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="12" builtinId="48"/>
-    <cellStyle name="强调文字颜色 2" xfId="13" builtinId="33"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="14" builtinId="32"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="15" builtinId="44"/>
-    <cellStyle name="计算" xfId="16" builtinId="22"/>
-    <cellStyle name="强调文字颜色 1" xfId="17" builtinId="29"/>
-    <cellStyle name="适中" xfId="18" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="19" builtinId="46"/>
-    <cellStyle name="好" xfId="20" builtinId="26"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="21" builtinId="30"/>
-    <cellStyle name="汇总" xfId="22" builtinId="25"/>
-    <cellStyle name="差" xfId="23" builtinId="27"/>
-    <cellStyle name="检查单元格" xfId="24" builtinId="23"/>
-    <cellStyle name="输出" xfId="25" builtinId="21"/>
-    <cellStyle name="标题 1" xfId="26" builtinId="16"/>
-    <cellStyle name="解释性文本" xfId="27" builtinId="53"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="28" builtinId="34"/>
-    <cellStyle name="标题 4" xfId="29" builtinId="19"/>
-    <cellStyle name="货币[0]" xfId="30" builtinId="7"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="31" builtinId="43"/>
-    <cellStyle name="千位分隔" xfId="32" builtinId="3"/>
-    <cellStyle name="已访问的超链接" xfId="33" builtinId="9"/>
-    <cellStyle name="标题" xfId="34" builtinId="15"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="35" builtinId="35"/>
-    <cellStyle name="警告文本" xfId="36" builtinId="11"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="37" builtinId="40"/>
-    <cellStyle name="注释" xfId="38" builtinId="10"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="39" builtinId="50"/>
-    <cellStyle name="强调文字颜色 5" xfId="40" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="41" builtinId="51"/>
-    <cellStyle name="超链接" xfId="42" builtinId="8"/>
-    <cellStyle name="千位分隔[0]" xfId="43" builtinId="6"/>
-    <cellStyle name="标题 2" xfId="44" builtinId="17"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="45" builtinId="47"/>
-    <cellStyle name="标题 3" xfId="46" builtinId="18"/>
-    <cellStyle name="强调文字颜色 6" xfId="47" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="48" builtinId="31"/>
-    <cellStyle name="链接单元格" xfId="49" builtinId="24"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="常规 2" xfId="49"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
@@ -3217,7 +3232,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="CCE8CF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -3465,7 +3480,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:H27"/>
   <sheetViews>
@@ -3473,155 +3488,155 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.2" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.25" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="15.5789473684211" style="6" customWidth="1"/>
-    <col min="2" max="2" width="10.3289473684211" style="7" customWidth="1"/>
-    <col min="3" max="3" width="28.0789473684211" customWidth="1"/>
-    <col min="4" max="4" width="35.3289473684211" style="2" customWidth="1"/>
-    <col min="5" max="5" width="38.5789473684211" customWidth="1"/>
-    <col min="6" max="6" width="23.4144736842105" customWidth="1"/>
-    <col min="7" max="7" width="21.5789473684211" customWidth="1"/>
+    <col min="1" max="1" width="15.5777777777778" style="7" customWidth="1"/>
+    <col min="2" max="2" width="10.3259259259259" style="8" customWidth="1"/>
+    <col min="3" max="3" width="28.0814814814815" customWidth="1"/>
+    <col min="4" max="4" width="35.3259259259259" style="5" customWidth="1"/>
+    <col min="5" max="5" width="38.5777777777778" customWidth="1"/>
+    <col min="6" max="6" width="23.4148148148148" customWidth="1"/>
+    <col min="7" max="7" width="21.5777777777778" customWidth="1"/>
     <col min="8" max="8" width="22" customWidth="1"/>
-    <col min="9" max="9" width="24.5789473684211" customWidth="1"/>
+    <col min="9" max="9" width="24.5777777777778" customWidth="1"/>
     <col min="10" max="10" width="27" customWidth="1"/>
-    <col min="11" max="11" width="19.0789473684211" customWidth="1"/>
-    <col min="12" max="12" width="18.5789473684211" customWidth="1"/>
-    <col min="13" max="13" width="13.0789473684211" customWidth="1"/>
-    <col min="14" max="1025" width="10.3289473684211" customWidth="1"/>
+    <col min="11" max="11" width="19.0814814814815" customWidth="1"/>
+    <col min="12" max="12" width="18.5777777777778" customWidth="1"/>
+    <col min="13" max="13" width="13.0814814814815" customWidth="1"/>
+    <col min="14" max="1025" width="10.3259259259259" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="64.5" customHeight="1" spans="1:8">
-      <c r="A1" s="8"/>
-      <c r="C1" s="9" t="s">
+      <c r="A1" s="9"/>
+      <c r="C1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-    </row>
-    <row r="2" spans="5:5">
-      <c r="E2" s="23"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+    </row>
+    <row r="2" ht="18" spans="5:5">
+      <c r="E2" s="12"/>
     </row>
     <row r="3" ht="49.5" customHeight="1" spans="3:7">
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="27" t="s">
+      <c r="D3" s="13"/>
+      <c r="E3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-    </row>
-    <row r="4" ht="16" spans="3:7">
-      <c r="C4" s="11" t="s">
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+    </row>
+    <row r="4" ht="18" spans="3:7">
+      <c r="C4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="28" t="s">
+      <c r="D4" s="15"/>
+      <c r="E4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="29" t="s">
+      <c r="F4" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="30" t="s">
+      <c r="G4" s="18" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" ht="16" spans="1:3">
-      <c r="A5" s="8"/>
+    <row r="5" spans="1:3">
+      <c r="A5" s="9"/>
       <c r="C5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="3:5">
-      <c r="C7" s="12" t="s">
+    <row r="7" ht="18" spans="3:5">
+      <c r="C7" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="21" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="3:5">
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="32"/>
-    </row>
-    <row r="9" ht="46" spans="3:6">
-      <c r="C9" s="16" t="s">
+      <c r="E8" s="24"/>
+    </row>
+    <row r="9" ht="51.75" spans="3:6">
+      <c r="C9" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="33" t="s">
+      <c r="E9" s="27" t="s">
         <v>15</v>
       </c>
       <c r="F9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" ht="46" spans="3:5">
-      <c r="C10" s="18" t="s">
+    <row r="10" ht="51.75" spans="3:5">
+      <c r="C10" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="33" t="s">
+      <c r="E10" s="27" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" ht="61" spans="3:5">
-      <c r="C11" s="14" t="s">
+    <row r="11" ht="69" spans="3:5">
+      <c r="C11" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="33" t="s">
+      <c r="E11" s="27" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" ht="16" spans="3:5">
-      <c r="C12" s="14" t="s">
+    <row r="12" spans="3:5">
+      <c r="C12" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="34" t="s">
+      <c r="E12" s="29" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="3:5">
-      <c r="C13" s="14"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="32"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="24"/>
     </row>
     <row r="14" spans="3:5">
-      <c r="C14" s="14"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="32"/>
-    </row>
-    <row r="15" ht="31" spans="3:5">
-      <c r="C15" s="19" t="s">
+      <c r="C14" s="22"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="24"/>
+    </row>
+    <row r="15" ht="34.5" spans="3:5">
+      <c r="C15" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="35" t="s">
+      <c r="E15" s="32" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3630,65 +3645,65 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" ht="16" spans="3:5">
-      <c r="C19" s="21" t="s">
+    <row r="19" spans="3:5">
+      <c r="C19" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-    </row>
-    <row r="20" ht="16" spans="3:4">
-      <c r="C20" s="22" t="s">
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+    </row>
+    <row r="20" ht="18" spans="3:4">
+      <c r="C20" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="23" t="s">
+      <c r="D20" s="12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" ht="16" spans="3:4">
-      <c r="C21" s="22" t="s">
+    <row r="21" ht="18" spans="3:4">
+      <c r="C21" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="23" t="s">
+      <c r="D21" s="12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" ht="16" spans="3:4">
-      <c r="C22" s="22" t="s">
+    <row r="22" ht="18" spans="3:4">
+      <c r="C22" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" ht="16" spans="3:4">
-      <c r="C23" s="22" t="s">
+    <row r="23" ht="18" spans="3:4">
+      <c r="C23" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="25" ht="69" customHeight="1" spans="3:5">
-      <c r="C25" s="24" t="s">
+      <c r="C25" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="10"/>
+      <c r="E25" s="13"/>
     </row>
     <row r="26" ht="14.25" customHeight="1" spans="3:5">
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E26" s="10"/>
-    </row>
-    <row r="27" ht="31" spans="3:3">
-      <c r="C27" s="25" t="s">
+      <c r="E26" s="13"/>
+    </row>
+    <row r="27" ht="51.75" spans="3:3">
+      <c r="C27" s="36" t="s">
         <v>43</v>
       </c>
     </row>
@@ -3709,25 +3724,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="E18" sqref="E18:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.25"/>
   <cols>
-    <col min="2" max="2" width="8.5" customWidth="1"/>
-    <col min="4" max="4" width="18.25" customWidth="1"/>
-    <col min="5" max="5" width="20.9144736842105" customWidth="1"/>
-    <col min="6" max="6" width="9.16447368421053" customWidth="1"/>
-    <col min="7" max="7" width="4.16447368421053" customWidth="1"/>
-    <col min="8" max="8" width="22.75" customWidth="1"/>
+    <col min="2" max="2" width="8.5037037037037" customWidth="1"/>
+    <col min="4" max="4" width="18.2518518518519" customWidth="1"/>
+    <col min="5" max="5" width="20.9111111111111" customWidth="1"/>
+    <col min="6" max="6" width="9.16296296296296" customWidth="1"/>
+    <col min="7" max="7" width="4.16296296296296" customWidth="1"/>
+    <col min="8" max="8" width="22.7481481481481" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="8.82894736842105" customWidth="1"/>
-    <col min="12" max="12" width="9.25" customWidth="1"/>
+    <col min="10" max="10" width="8.82962962962963" customWidth="1"/>
+    <col min="12" max="12" width="9.25185185185185" customWidth="1"/>
     <col min="13" max="13" width="30" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3746,291 +3761,291 @@
       </c>
     </row>
     <row r="4" spans="5:7">
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" ht="16" spans="1:13">
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K7" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="L7" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="M7" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="8" ht="16" spans="5:13">
-      <c r="E8" s="2" t="s">
+    <row r="8" spans="5:13">
+      <c r="E8" s="5" t="s">
         <v>63</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="5" t="s">
         <v>67</v>
       </c>
       <c r="K8">
         <v>1</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="L8" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="M8" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="9" ht="16" spans="5:13">
-      <c r="E9" s="2" t="s">
+    <row r="9" spans="5:13">
+      <c r="E9" s="5" t="s">
         <v>70</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="5" t="s">
         <v>67</v>
       </c>
       <c r="K9">
         <v>1</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="L9" s="5" t="s">
         <v>68</v>
       </c>
       <c r="M9" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="10" ht="16" spans="5:13">
-      <c r="E10" s="2" t="s">
+    <row r="10" spans="5:13">
+      <c r="E10" s="5" t="s">
         <v>74</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="5" t="s">
         <v>67</v>
       </c>
       <c r="K10">
         <v>1</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="L10" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="M10" s="5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="11" ht="16" spans="5:13">
-      <c r="E11" s="2" t="s">
+    <row r="11" spans="5:13">
+      <c r="E11" s="5" t="s">
         <v>78</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" s="5" t="s">
         <v>67</v>
       </c>
       <c r="K11">
         <v>1</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="L11" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="M11" s="2" t="s">
+      <c r="M11" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="12" ht="16" spans="5:13">
-      <c r="E12" s="2" t="s">
+    <row r="12" spans="5:13">
+      <c r="E12" s="5" t="s">
         <v>82</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I12" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" s="5" t="s">
         <v>67</v>
       </c>
       <c r="K12">
         <v>1</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="L12" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="M12" s="2" t="s">
+      <c r="M12" s="5" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="13" ht="16" spans="5:13">
-      <c r="E13" s="2" t="s">
+    <row r="13" spans="5:13">
+      <c r="E13" s="5" t="s">
         <v>86</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" s="5" t="s">
         <v>67</v>
       </c>
       <c r="K13">
         <v>1</v>
       </c>
-      <c r="L13" s="2" t="s">
+      <c r="L13" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="M13" s="2" t="s">
+      <c r="M13" s="5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="14" ht="16" spans="5:13">
-      <c r="E14" s="2" t="s">
+    <row r="14" spans="5:13">
+      <c r="E14" s="5" t="s">
         <v>90</v>
       </c>
       <c r="F14">
         <v>0</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I14" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J14" s="5" t="s">
         <v>67</v>
       </c>
       <c r="K14">
         <v>1</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="L14" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="M14" s="2" t="s">
+      <c r="M14" s="5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="15" ht="16" spans="5:13">
-      <c r="E15" s="2" t="s">
+    <row r="15" spans="5:13">
+      <c r="E15" s="5" t="s">
         <v>94</v>
       </c>
       <c r="F15">
         <v>0</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="I15" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="J15" s="5" t="s">
         <v>67</v>
       </c>
       <c r="K15">
         <v>1</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="L15" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="M15" s="2" t="s">
+      <c r="M15" s="5" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="16" spans="5:13">
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="5" t="s">
         <v>98</v>
       </c>
       <c r="F16">
@@ -4059,7 +4074,7 @@
       </c>
     </row>
     <row r="17" spans="5:13">
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="5" t="s">
         <v>103</v>
       </c>
       <c r="F17">
@@ -4088,16 +4103,16 @@
       </c>
     </row>
     <row r="18" spans="2:13">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="5" t="s">
         <v>107</v>
       </c>
       <c r="F18">
         <v>0</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="3" t="s">
         <v>99</v>
       </c>
       <c r="H18" t="s">
@@ -4119,50 +4134,75 @@
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="5:7">
-      <c r="E19" s="2"/>
-      <c r="G19" s="2"/>
+    <row r="19" spans="5:13">
+      <c r="E19" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="I19" t="s">
+        <v>113</v>
+      </c>
+      <c r="J19" t="s">
+        <v>67</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19" t="s">
+        <v>68</v>
+      </c>
+      <c r="M19" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="20" spans="5:7">
-      <c r="E20" s="2"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="2"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="5"/>
     </row>
     <row r="21" spans="5:7">
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
     </row>
     <row r="22" spans="5:7">
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
     </row>
     <row r="23" spans="5:7">
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
     </row>
     <row r="24" spans="5:7">
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
     </row>
     <row r="25" spans="5:7">
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
     </row>
     <row r="26" spans="5:7">
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
     </row>
     <row r="27" spans="6:6">
-      <c r="F27" s="2"/>
+      <c r="F27" s="5"/>
     </row>
     <row r="28" spans="6:6">
-      <c r="F28" s="2"/>
+      <c r="F28" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>